<commit_message>
Initial commit for online alumni portal Flask app
</commit_message>
<xml_diff>
--- a/static/Alumni_email_static_Data.xlsx
+++ b/static/Alumni_email_static_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shrav\OneDrive\Desktop\TY Project\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77078FC-6B6C-4A04-9A50-43DE71720353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4CDD4E-90ED-4D1B-9582-B05C7A604AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C8DBA018-57F7-42A6-9C4D-53A56DFFF9A4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t xml:space="preserve">                                                                                 Alumni Portal Data students and alumni</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>rakesh_patil25@gmail.com</t>
+  </si>
+  <si>
+    <t>rakesh147</t>
+  </si>
+  <si>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>hemant_patil@gmail.com</t>
+  </si>
+  <si>
+    <t>hemantpatil147</t>
   </si>
 </sst>
 </file>
@@ -471,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30633B0-8C56-41B8-9641-82DAB751C0AF}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,6 +577,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{FBEC3EB7-34B2-4A31-8E03-E66C70E951E1}"/>
@@ -569,6 +606,8 @@
     <hyperlink ref="A5" r:id="rId3" xr:uid="{1AD4D221-A52C-4723-9655-57F9BB273147}"/>
     <hyperlink ref="A6" r:id="rId4" xr:uid="{340DEE9E-5CE1-43E6-9C49-41805CB24F64}"/>
     <hyperlink ref="A7" r:id="rId5" xr:uid="{CED270C8-4945-4AB0-9A80-CC2F40FDB2FA}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{D67D3AED-8955-414D-A2D1-F843B796CDF4}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{E4CFFC19-2E46-4CF4-AF08-061FAE857E66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>